<commit_message>
report agent를 tool로 만들기 완료
</commit_message>
<xml_diff>
--- a/report_agent/output/predicted_quarterly_financial_data/005930_predicted_quarter_financial_data.xlsx
+++ b/report_agent/output/predicted_quarterly_financial_data/005930_predicted_quarter_financial_data.xlsx
@@ -517,7 +517,7 @@
         <v>80965200000000</v>
       </c>
       <c r="G3" t="n">
-        <v>123199825000000</v>
+        <v>79913400000000</v>
       </c>
     </row>
     <row r="4">
@@ -592,7 +592,7 @@
         <v>225082634000000</v>
       </c>
       <c r="G6" t="n">
-        <v>342670240950000</v>
+        <v>299383815950000</v>
       </c>
     </row>
     <row r="7">
@@ -617,7 +617,7 @@
         <v>26233258000000</v>
       </c>
       <c r="G7" t="n">
-        <v>39938029336210.43</v>
+        <v>34893020155614.79</v>
       </c>
     </row>
     <row r="8">
@@ -642,7 +642,7 @@
         <v>26696957000000</v>
       </c>
       <c r="G8" t="n">
-        <v>40643973838611.6</v>
+        <v>35509789088895.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>